<commit_message>
Ajuste en escaleta Mat 7 tema 5
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion05/Escaleta MA_07_05_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion05/Escaleta MA_07_05_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="262">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1125,13 +1130,22 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1171,15 +1185,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1242,7 +1247,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1277,7 +1282,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1489,8 +1494,8 @@
   <dimension ref="A1:U283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,94 +1524,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="57"/>
+      <c r="O1" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="58" t="s">
+      <c r="S1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="U1" s="43" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="49"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="13" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="58"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1648,7 +1653,9 @@
       <c r="O3" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="P3" s="22"/>
+      <c r="P3" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q3" s="38">
         <v>6</v>
       </c>
@@ -1701,7 +1708,9 @@
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="24"/>
-      <c r="P4" s="22"/>
+      <c r="P4" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q4" s="38">
         <v>8</v>
       </c>
@@ -1758,7 +1767,9 @@
       <c r="O5" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="P5" s="22"/>
+      <c r="P5" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q5" s="38">
         <v>6</v>
       </c>
@@ -1813,7 +1824,9 @@
       <c r="O6" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="P6" s="22"/>
+      <c r="P6" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q6" s="38">
         <v>6</v>
       </c>
@@ -1870,7 +1883,9 @@
       <c r="O7" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="P7" s="22"/>
+      <c r="P7" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q7" s="38">
         <v>6</v>
       </c>
@@ -1923,7 +1938,9 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="22"/>
+      <c r="P8" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q8" s="38">
         <v>8</v>
       </c>
@@ -1980,7 +1997,9 @@
       <c r="O9" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="P9" s="22"/>
+      <c r="P9" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q9" s="38">
         <v>6</v>
       </c>
@@ -2037,7 +2056,9 @@
         <v>121</v>
       </c>
       <c r="O10" s="24"/>
-      <c r="P10" s="22"/>
+      <c r="P10" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q10" s="38">
         <v>6</v>
       </c>
@@ -2090,7 +2111,9 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="24"/>
-      <c r="P11" s="22"/>
+      <c r="P11" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q11" s="38">
         <v>5</v>
       </c>
@@ -2145,7 +2168,9 @@
         <v>118</v>
       </c>
       <c r="O12" s="24"/>
-      <c r="P12" s="22"/>
+      <c r="P12" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q12" s="38">
         <v>6</v>
       </c>
@@ -2202,7 +2227,9 @@
       <c r="O13" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="P13" s="22"/>
+      <c r="P13" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="Q13" s="38">
         <v>6</v>
       </c>
@@ -2259,7 +2286,9 @@
         <v>121</v>
       </c>
       <c r="O14" s="19"/>
-      <c r="P14" s="22"/>
+      <c r="P14" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q14" s="38">
         <v>6</v>
       </c>
@@ -2312,7 +2341,9 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="22"/>
+      <c r="P15" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q15" s="38">
         <v>8</v>
       </c>
@@ -2365,7 +2396,9 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="24"/>
-      <c r="P16" s="22"/>
+      <c r="P16" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q16" s="38">
         <v>8</v>
       </c>
@@ -2422,7 +2455,9 @@
       <c r="O17" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="P17" s="22"/>
+      <c r="P17" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="Q17" s="38">
         <v>6</v>
       </c>
@@ -2479,7 +2514,9 @@
       <c r="O18" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="P18" s="22"/>
+      <c r="P18" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q18" s="38">
         <v>6</v>
       </c>
@@ -2536,7 +2573,9 @@
         <v>121</v>
       </c>
       <c r="O19" s="19"/>
-      <c r="P19" s="22"/>
+      <c r="P19" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q19" s="38">
         <v>6</v>
       </c>
@@ -2593,7 +2632,9 @@
       <c r="O20" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="P20" s="22"/>
+      <c r="P20" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q20" s="38">
         <v>6</v>
       </c>
@@ -2646,7 +2687,9 @@
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="24"/>
-      <c r="P21" s="22"/>
+      <c r="P21" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q21" s="38">
         <v>8</v>
       </c>
@@ -2699,7 +2742,9 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="24"/>
-      <c r="P22" s="22"/>
+      <c r="P22" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q22" s="38">
         <v>8</v>
       </c>
@@ -2756,7 +2801,9 @@
       <c r="O23" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="P23" s="22"/>
+      <c r="P23" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="Q23" s="38">
         <v>6</v>
       </c>
@@ -2815,7 +2862,9 @@
       <c r="O24" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="P24" s="22"/>
+      <c r="P24" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q24" s="38">
         <v>6</v>
       </c>
@@ -2868,7 +2917,9 @@
       <c r="M25" s="7"/>
       <c r="N25" s="14"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="22"/>
+      <c r="P25" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q25" s="38">
         <v>6</v>
       </c>
@@ -2925,7 +2976,9 @@
       <c r="O26" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="P26" s="22"/>
+      <c r="P26" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="Q26" s="38">
         <v>6</v>
       </c>
@@ -2982,7 +3035,9 @@
       <c r="O27" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="P27" s="22"/>
+      <c r="P27" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q27" s="38">
         <v>6</v>
       </c>
@@ -3039,7 +3094,9 @@
         <v>121</v>
       </c>
       <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
+      <c r="P28" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q28" s="38">
         <v>6</v>
       </c>
@@ -3094,7 +3151,9 @@
         <v>41</v>
       </c>
       <c r="O29" s="19"/>
-      <c r="P29" s="22"/>
+      <c r="P29" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q29" s="38">
         <v>6</v>
       </c>
@@ -3151,7 +3210,9 @@
       <c r="O30" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="P30" s="22"/>
+      <c r="P30" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q30" s="38">
         <v>6</v>
       </c>
@@ -3210,7 +3271,9 @@
       <c r="O31" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="P31" s="22"/>
+      <c r="P31" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q31" s="38">
         <v>6</v>
       </c>
@@ -3263,7 +3326,9 @@
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="19"/>
-      <c r="P32" s="22"/>
+      <c r="P32" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q32" s="38">
         <v>8</v>
       </c>
@@ -3318,7 +3383,9 @@
       <c r="O33" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="22"/>
+      <c r="P33" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q33" s="38">
         <v>8</v>
       </c>
@@ -3375,7 +3442,9 @@
       <c r="O34" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="P34" s="22"/>
+      <c r="P34" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q34" s="38">
         <v>6</v>
       </c>
@@ -3434,7 +3503,9 @@
       <c r="O35" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="P35" s="22"/>
+      <c r="P35" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q35" s="38">
         <v>6</v>
       </c>
@@ -3487,7 +3558,9 @@
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
       <c r="O36" s="19"/>
-      <c r="P36" s="22"/>
+      <c r="P36" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q36" s="38">
         <v>8</v>
       </c>
@@ -3542,7 +3615,9 @@
       <c r="O37" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="P37" s="22"/>
+      <c r="P37" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q37" s="38">
         <v>8</v>
       </c>
@@ -3595,7 +3670,9 @@
       <c r="M38" s="7"/>
       <c r="N38" s="7"/>
       <c r="O38" s="19"/>
-      <c r="P38" s="22"/>
+      <c r="P38" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q38" s="38"/>
       <c r="R38" s="39"/>
       <c r="S38" s="38"/>
@@ -3640,7 +3717,9 @@
         <v>33</v>
       </c>
       <c r="O39" s="19"/>
-      <c r="P39" s="22"/>
+      <c r="P39" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="Q39" s="38">
         <v>6</v>
       </c>
@@ -3695,7 +3774,9 @@
       <c r="O40" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="P40" s="22"/>
+      <c r="P40" s="23" t="s">
+        <v>20</v>
+      </c>
       <c r="Q40" s="38">
         <v>6</v>
       </c>
@@ -4742,12 +4823,6 @@
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4762,6 +4837,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4784,7 +4865,7 @@
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I69 P29:P69 P3:P27 K3:K69</xm:sqref>
+          <xm:sqref>I3:I69 K3:K69 P3:P69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Escaletas ubicadas en git hub
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion05/Escaleta MA_07_05_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion05/Escaleta MA_07_05_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion05\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -13,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="263">
   <si>
     <t>Asignatura</t>
   </si>
@@ -805,6 +810,9 @@
   </si>
   <si>
     <t>Recurso M101A-05</t>
+  </si>
+  <si>
+    <t>Clara Melo</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1125,13 +1133,22 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1173,15 +1190,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1242,7 +1251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1277,7 +1286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1486,11 +1495,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U283"/>
+  <dimension ref="A1:W283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X42" sqref="X42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,12 +1513,12 @@
     <col min="7" max="7" width="69.42578125" style="20" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="30" customWidth="1"/>
     <col min="9" max="9" width="11" style="30" customWidth="1"/>
-    <col min="10" max="10" width="78.42578125" style="20" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="78.42578125" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="20" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="37.85546875" style="30" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="30" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="30" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" style="30" customWidth="1"/>
     <col min="18" max="18" width="23" style="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" style="20" bestFit="1" customWidth="1"/>
@@ -1518,97 +1527,97 @@
     <col min="22" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:23" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="57"/>
+      <c r="O1" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="58" t="s">
+      <c r="S1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="U1" s="43" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="49"/>
+    <row r="2" spans="1:23" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="13" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="58"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="43"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
@@ -1666,8 +1675,14 @@
       <c r="U3" s="38" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V3" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W3" s="61">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -1780,8 +1795,14 @@
       <c r="U5" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V5" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W5" s="61">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1838,7 +1859,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1896,8 +1917,14 @@
       <c r="U7" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V7" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W7" s="61">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -1952,7 +1979,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
@@ -2010,8 +2037,14 @@
       <c r="U9" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V9" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W9" s="61">
+        <v>37987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -2069,8 +2102,14 @@
       <c r="U10" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V10" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W10" s="61">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
@@ -2125,7 +2164,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -2181,8 +2220,14 @@
       <c r="U12" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V12" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W12" s="61">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -2240,8 +2285,14 @@
       <c r="U13" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V13" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W13" s="61">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2299,8 +2350,14 @@
       <c r="U14" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V14" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W14" s="61">
+        <v>38353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
@@ -2355,7 +2412,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
@@ -2410,7 +2467,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2468,8 +2525,14 @@
       <c r="U17" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V17" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W17" s="61">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2527,8 +2590,14 @@
       <c r="U18" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V18" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W18" s="61">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
@@ -2586,8 +2655,14 @@
       <c r="U19" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V19" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W19" s="61">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
@@ -2645,8 +2720,14 @@
       <c r="U20" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V20" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W20" s="61">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -2701,7 +2782,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>15</v>
       </c>
@@ -2756,7 +2837,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -2814,8 +2895,14 @@
       <c r="U23" s="38" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V23" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W23" s="61">
+        <v>39814</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -2875,8 +2962,11 @@
       <c r="U24" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V24" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
@@ -2931,7 +3021,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
@@ -2989,8 +3079,14 @@
       <c r="U26" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V26" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W26" s="61">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
@@ -3048,8 +3144,14 @@
       <c r="U27" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V27" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W27" s="61">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>15</v>
       </c>
@@ -3107,8 +3209,14 @@
       <c r="U28" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V28" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W28" s="61">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
@@ -3164,8 +3272,14 @@
       <c r="U29" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V29" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W29" s="61">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>15</v>
       </c>
@@ -3223,8 +3337,14 @@
       <c r="U30" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V30" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W30" s="61">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>15</v>
       </c>
@@ -3284,8 +3404,14 @@
       <c r="U31" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V31" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W31" s="61">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>15</v>
       </c>
@@ -3340,7 +3466,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>15</v>
       </c>
@@ -3397,7 +3523,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>15</v>
       </c>
@@ -3455,8 +3581,14 @@
       <c r="U34" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V34" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W34" s="61">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>15</v>
       </c>
@@ -3516,8 +3648,14 @@
       <c r="U35" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V35" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W35" s="61">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>15</v>
       </c>
@@ -3572,7 +3710,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>15</v>
       </c>
@@ -3629,7 +3767,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>15</v>
       </c>
@@ -3674,7 +3812,7 @@
       <c r="T38" s="41"/>
       <c r="U38" s="38"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>15</v>
       </c>
@@ -3730,8 +3868,14 @@
       <c r="U39" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V39" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W39" s="61">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>15</v>
       </c>
@@ -3787,8 +3931,14 @@
       <c r="U40" s="38" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V40" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="W40" s="61">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="21"/>
       <c r="C41" s="35"/>
@@ -3811,7 +3961,7 @@
       <c r="T41" s="33"/>
       <c r="U41" s="31"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="21"/>
       <c r="C42" s="35"/>
@@ -3834,7 +3984,7 @@
       <c r="T42" s="33"/>
       <c r="U42" s="31"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="21"/>
       <c r="C43" s="35"/>
@@ -3857,7 +4007,7 @@
       <c r="T43" s="33"/>
       <c r="U43" s="31"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="21"/>
       <c r="C44" s="35"/>
@@ -3880,7 +4030,7 @@
       <c r="T44" s="33"/>
       <c r="U44" s="31"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="21"/>
       <c r="C45" s="35"/>
@@ -3903,7 +4053,7 @@
       <c r="T45" s="33"/>
       <c r="U45" s="31"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="21"/>
       <c r="C46" s="35"/>
@@ -3926,7 +4076,7 @@
       <c r="T46" s="33"/>
       <c r="U46" s="31"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="21"/>
       <c r="C47" s="35"/>
@@ -3949,7 +4099,7 @@
       <c r="T47" s="33"/>
       <c r="U47" s="31"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="21"/>
       <c r="C48" s="35"/>
@@ -4818,12 +4968,6 @@
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4838,6 +4982,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>